<commit_message>
documentatie geupdate en georderd + film toevoegen functie af
leader en notitie documenten geupdate en georderd + film toevoegen functie af
</commit_message>
<xml_diff>
--- a/leader_schema.xlsx
+++ b/leader_schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc-janiek\Documents\Git_Repository\leerjaar2\bioscoop\bioscoop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629BEC77-A559-45A1-9FD6-07B6389D4D73}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2A952D-357B-4FCC-99DC-2DCF459051CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{D7922EC9-7A18-4D9E-ADED-83595DB6342A}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,10 +510,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>